<commit_message>
AIP-1641 AIP-1643 updated 4U3U file as per review comments
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/4U3U.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/4U3U.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F0B5E6-72E9-4609-AC86-3DE83DC699A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9E607F-093A-49B6-A073-68A5EED6F809}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -739,7 +739,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DD3A37-1E65-4B23-B52F-328312BA3BC2}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +801,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
         <v>124</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>